<commit_message>
looks thru a defined rage, and finds a fund and a variant. Adds fund and variant to dictionary if logic is met. Prints dicionary into cells of active worksheet.
</commit_message>
<xml_diff>
--- a/FileFolder/1.xlsx
+++ b/FileFolder/1.xlsx
@@ -23,6 +23,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>fund</t>
+  </si>
+  <si>
+    <t>NAV per</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>BM tol</t>
+  </si>
+  <si>
+    <t>BM Bps Var</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
@@ -34,12 +54,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -54,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,20 +364,340 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>3123</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2">
+        <v>130</v>
+      </c>
+      <c r="N2">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1">
+        <f t="shared" ref="O2:O9" si="0">M2-L2</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>3123</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>130</v>
+      </c>
+      <c r="N3">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>3123</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4">
+        <v>130</v>
+      </c>
+      <c r="N4">
+        <v>20</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>3456</v>
+      </c>
+      <c r="L5">
+        <v>120</v>
+      </c>
+      <c r="M5">
+        <v>110</v>
+      </c>
+      <c r="N5">
+        <v>40</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>3456</v>
+      </c>
+      <c r="L6">
+        <v>120</v>
+      </c>
+      <c r="M6">
+        <v>110</v>
+      </c>
+      <c r="N6">
+        <v>40</v>
+      </c>
+      <c r="O6">
+        <f>M6-L6</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>3478</v>
+      </c>
+      <c r="L7">
+        <v>-60</v>
+      </c>
+      <c r="M7">
+        <v>-10</v>
+      </c>
+      <c r="N7">
+        <v>30</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>3478</v>
+      </c>
+      <c r="L8">
+        <v>-60</v>
+      </c>
+      <c r="M8">
+        <v>-10</v>
+      </c>
+      <c r="N8">
+        <v>30</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>3969</v>
+      </c>
+      <c r="L9">
+        <v>-70</v>
+      </c>
+      <c r="M9">
+        <v>-60</v>
+      </c>
+      <c r="N9">
+        <v>30</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>3478</v>
+      </c>
+      <c r="L10">
+        <v>-60</v>
+      </c>
+      <c r="M10">
+        <v>-10</v>
+      </c>
+      <c r="N10">
+        <v>30</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" ref="O10:O18" si="1">M10-L10</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>3478</v>
+      </c>
+      <c r="L11">
+        <v>-60</v>
+      </c>
+      <c r="M11">
+        <v>-10</v>
+      </c>
+      <c r="N11">
+        <v>30</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>3969</v>
+      </c>
+      <c r="L12">
+        <v>-70</v>
+      </c>
+      <c r="M12">
+        <v>-60</v>
+      </c>
+      <c r="N12">
+        <v>30</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>3478</v>
+      </c>
+      <c r="L13">
+        <v>-60</v>
+      </c>
+      <c r="M13">
+        <v>-10</v>
+      </c>
+      <c r="N13">
+        <v>30</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>3478</v>
+      </c>
+      <c r="L14">
+        <v>-60</v>
+      </c>
+      <c r="M14">
+        <v>-10</v>
+      </c>
+      <c r="N14">
+        <v>30</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>3969</v>
+      </c>
+      <c r="L15">
+        <v>-70</v>
+      </c>
+      <c r="M15">
+        <v>-60</v>
+      </c>
+      <c r="N15">
+        <v>30</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>234</v>
+      </c>
+      <c r="L16">
+        <v>-60</v>
+      </c>
+      <c r="M16">
+        <v>-10</v>
+      </c>
+      <c r="N16">
+        <v>30</v>
+      </c>
+      <c r="O16" s="1">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>-60</v>
+      </c>
+      <c r="M17">
+        <v>-10</v>
+      </c>
+      <c r="N17">
+        <v>30</v>
+      </c>
+      <c r="O17" s="1">
+        <v>1231231</v>
+      </c>
+    </row>
+    <row r="18" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>11</v>
+      </c>
+      <c r="L18">
+        <v>-70</v>
+      </c>
+      <c r="M18">
+        <v>-60</v>
+      </c>
+      <c r="N18">
+        <v>30</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>